<commit_message>
03/20/2025 FIXED EVERYTHING NA! Yung pagination gawa ka na lang ng Css Style mo :D Godbless
</commit_message>
<xml_diff>
--- a/HelpDeskVG/ReportFiles/AUTOCLOSEDTICKETS.xlsx
+++ b/HelpDeskVG/ReportFiles/AUTOCLOSEDTICKETS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SOLID FIVE\source\repos\HelpDeskVG\HelpDeskVG\ReportFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5FCF8FB-C591-4DA5-A0D9-1051224769C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{410C4CAC-F2BF-4253-900F-3382A5344431}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2625" yWindow="7170" windowWidth="22200" windowHeight="8685" xr2:uid="{F7C88789-CF15-4FCD-8AF8-A29C54CC2541}"/>
+    <workbookView xWindow="3825" yWindow="2190" windowWidth="22200" windowHeight="9810" xr2:uid="{F7C88789-CF15-4FCD-8AF8-A29C54CC2541}"/>
   </bookViews>
   <sheets>
     <sheet name="AutoClosedTicket" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>AUTO CLOSED TICKETS</t>
   </si>
@@ -78,6 +78,12 @@
   </si>
   <si>
     <t>WITH THIRD PARTY?</t>
+  </si>
+  <si>
+    <t>SUBJECT</t>
+  </si>
+  <si>
+    <t>DESCRIPTION</t>
   </si>
 </sst>
 </file>
@@ -456,35 +462,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13932EC1-4E93-47B3-9C4E-A7826433162B}">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.85546875" customWidth="1"/>
     <col min="2" max="2" width="15.85546875" customWidth="1"/>
-    <col min="3" max="3" width="21.28515625" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" customWidth="1"/>
-    <col min="5" max="5" width="26.42578125" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" customWidth="1"/>
-    <col min="9" max="9" width="20.140625" customWidth="1"/>
-    <col min="10" max="10" width="17.140625" customWidth="1"/>
-    <col min="11" max="11" width="25.85546875" customWidth="1"/>
-    <col min="12" max="12" width="31.5703125" customWidth="1"/>
-    <col min="13" max="13" width="21" customWidth="1"/>
+    <col min="3" max="3" width="26.5703125" customWidth="1"/>
+    <col min="4" max="4" width="32.42578125" customWidth="1"/>
+    <col min="5" max="5" width="21.28515625" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" customWidth="1"/>
+    <col min="7" max="7" width="26.42578125" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" customWidth="1"/>
+    <col min="11" max="11" width="20.140625" customWidth="1"/>
+    <col min="12" max="12" width="17.140625" customWidth="1"/>
+    <col min="13" max="13" width="25.85546875" customWidth="1"/>
+    <col min="14" max="14" width="31.5703125" customWidth="1"/>
+    <col min="15" max="15" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -492,36 +500,42 @@
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="M4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="N4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="O4" s="1" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
06/11/2025 Fixed Showing up of Draft Button for IT PIC (Accepted Tix)
</commit_message>
<xml_diff>
--- a/HelpDeskVG/ReportFiles/AUTOCLOSEDTICKETS.xlsx
+++ b/HelpDeskVG/ReportFiles/AUTOCLOSEDTICKETS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SOLID FIVE\source\repos\HelpDeskVG\HelpDeskVG\ReportFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{410C4CAC-F2BF-4253-900F-3382A5344431}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2BA0693-122D-4719-8577-4D71F006B168}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3825" yWindow="2190" windowWidth="22200" windowHeight="9810" xr2:uid="{F7C88789-CF15-4FCD-8AF8-A29C54CC2541}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F7C88789-CF15-4FCD-8AF8-A29C54CC2541}"/>
   </bookViews>
   <sheets>
     <sheet name="AutoClosedTicket" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>AUTO CLOSED TICKETS</t>
   </si>
@@ -84,12 +84,33 @@
   </si>
   <si>
     <t>DESCRIPTION</t>
+  </si>
+  <si>
+    <t>ASSIGNED IT PIC</t>
+  </si>
+  <si>
+    <t>ASSIGNED DATE TIME</t>
+  </si>
+  <si>
+    <t>RESOLVED DATE TIME</t>
+  </si>
+  <si>
+    <t>SLA HOURS</t>
+  </si>
+  <si>
+    <t>ACTUAL HOURS</t>
+  </si>
+  <si>
+    <t>HIT OR MISS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="mm/dd/yyyy\ hh:mm\ AM/PM"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -125,9 +146,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -462,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13932EC1-4E93-47B3-9C4E-A7826433162B}">
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:U4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -485,14 +507,20 @@
     <col min="13" max="13" width="25.85546875" customWidth="1"/>
     <col min="14" max="14" width="31.5703125" customWidth="1"/>
     <col min="15" max="15" width="21" customWidth="1"/>
+    <col min="16" max="16" width="26.7109375" customWidth="1"/>
+    <col min="17" max="17" width="31.7109375" customWidth="1"/>
+    <col min="18" max="18" width="28.42578125" customWidth="1"/>
+    <col min="19" max="19" width="27.85546875" customWidth="1"/>
+    <col min="20" max="20" width="26.85546875" customWidth="1"/>
+    <col min="21" max="21" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -537,6 +565,24 @@
       </c>
       <c r="O4" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>